<commit_message>
add more RDS and fix juvenile excretion
</commit_message>
<xml_diff>
--- a/Master_Data/literature_extraction.xlsx
+++ b/Master_Data/literature_extraction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jo\OneDrive\Documents\GitHub\Species-Traits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8365a1eecae1c53e/Documents/GitHub/Species-Traits/Master_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3630" documentId="8_{8303F361-5CFA-49CF-93EB-E47B0D017CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0AEAFDC1-1549-49FC-981C-81107BBD03C9}"/>
+  <xr:revisionPtr revIDLastSave="3631" documentId="8_{8303F361-5CFA-49CF-93EB-E47B0D017CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{86674587-1F5B-42EA-8B1D-BABD3FABA7E5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{163C3060-5853-4BB6-B46C-A85E56A5A6D8}"/>
+    <workbookView xWindow="1005" yWindow="0" windowWidth="22635" windowHeight="12510" activeTab="1" xr2:uid="{163C3060-5853-4BB6-B46C-A85E56A5A6D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4221,7 +4223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4942DADD-73DC-45E2-A058-0029641B6054}">
   <dimension ref="A1:G298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
+    <sheetView topLeftCell="A281" workbookViewId="0">
       <selection activeCell="E290" sqref="E290"/>
     </sheetView>
   </sheetViews>
@@ -9382,13 +9384,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C553106-9EFB-4C5F-86D3-BA2759CF7F90}">
   <dimension ref="A1:BP344"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AW78" sqref="AW78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="7" max="7" width="15" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
     <col min="21" max="21" width="15.85546875" customWidth="1"/>

</xml_diff>